<commit_message>
journal + creation doc fonctionnement de l'application
</commit_message>
<xml_diff>
--- a/Android/regle de nommage.xlsx
+++ b/Android/regle de nommage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Regle de nommage</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>layout-small/chrono_frag_affichage.xml</t>
+  </si>
+  <si>
+    <t>EditionExerciceActivity</t>
+  </si>
+  <si>
+    <t>autre</t>
+  </si>
+  <si>
+    <t>ChronoService</t>
+  </si>
+  <si>
+    <t>ListeSonsActivity</t>
+  </si>
+  <si>
+    <t>EditionExercicePlaylistActivity</t>
   </si>
 </sst>
 </file>
@@ -575,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -609,338 +624,369 @@
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="D7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="D9" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="D10" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
+      <c r="D12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="D13" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="D22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="D16" t="s">
+    <row r="23" spans="2:4">
+      <c r="D23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
-      <c r="D17" t="s">
+    <row r="24" spans="2:4">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
-      <c r="D18" t="s">
+    <row r="25" spans="2:4">
+      <c r="D25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
-      <c r="D19" t="s">
+    <row r="26" spans="2:4">
+      <c r="D26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
-      <c r="D20" t="s">
+    <row r="27" spans="2:4">
+      <c r="D27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
-      <c r="C21" t="s">
+    <row r="28" spans="2:4">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
-      <c r="D22" t="s">
+    <row r="29" spans="2:4">
+      <c r="D29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
-      <c r="D23" t="s">
+    <row r="30" spans="2:4">
+      <c r="D30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
-      <c r="D24" t="s">
+    <row r="31" spans="2:4">
+      <c r="D31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="3:4">
-      <c r="C25" t="s">
+    <row r="32" spans="2:4">
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4">
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4">
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4">
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4">
-      <c r="D29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4">
-      <c r="D30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4">
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4">
-      <c r="D32" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="D33" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>37</v>
+      <c r="D34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="D35" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="D36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="D40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="D43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B48" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="C42" t="s">
+    <row r="49" spans="2:3">
+      <c r="C49" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="C44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="C45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="C46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="C47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="C50" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="C51" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="C52" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="2:3">
-      <c r="B53" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>57</v>
+      <c r="C53" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="C54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="C55" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="C57" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="C58" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="C59" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="C60" t="s">
-        <v>63</v>
+      <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="C61" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="C62" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="2:3">
-      <c r="C63" t="s">
-        <v>66</v>
+      <c r="B63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="C64" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="D6:D13">
+    <sortCondition ref="D6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>